<commit_message>
modified the strategy to 1 and -1 MACD
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_MACD.xlsx
+++ b/Data/binance_ETHUSDT_MACD.xlsx
@@ -467,7 +467,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>134.65000000</t>
+          <t>137.50000000</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -477,12 +477,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>131.06000000</t>
+          <t>130.71000000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>220536.94136000</t>
+          <t>364019.63667000</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -490,20 +490,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>28689211.19842310</t>
+          <t>47857523.46199840</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>56036</v>
+        <v>95415</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>123092.37361000</t>
+          <t>194328.98558000</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>16011979.34768310</t>
+          <t>25538041.77371310</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -522,13 +522,13 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>-0.7565568594104519</v>
+        <v>-0.7844770873306572</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.1144879785358383</v>
+        <v>0.1089039329517972</v>
       </c>
       <c r="R2" t="n">
-        <v>-0.8710448379462902</v>
+        <v>-0.8933810202824545</v>
       </c>
     </row>
     <row r="3">

</xml_diff>

<commit_message>
20200920 Update missing sell signal
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_MACD.xlsx
+++ b/Data/binance_ETHUSDT_MACD.xlsx
@@ -507,12 +507,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>366.51000000</t>
+          <t>367.10000000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>31731.04207000</t>
+          <t>41055.15480000</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -520,20 +520,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>11691983.83048400</t>
+          <t>15116722.51812100</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>12047</v>
+        <v>15912</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>14205.40739000</t>
+          <t>18723.93841000</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>5233799.51044640</t>
+          <t>6893569.95812560</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -552,22 +552,22 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>-0.2122777601587131</v>
+        <v>-0.1652122330932002</v>
       </c>
       <c r="Q2" t="n">
-        <v>1.949882174491122</v>
+        <v>1.959295279904225</v>
       </c>
       <c r="R2" t="n">
-        <v>-2.162159934649835</v>
+        <v>-2.124507512997425</v>
       </c>
       <c r="S2" t="n">
-        <v>3.65587038798941</v>
+        <v>3.735642467761522</v>
       </c>
       <c r="T2" t="n">
-        <v>2.723511804120747</v>
+        <v>2.739466220075169</v>
       </c>
       <c r="U2" t="n">
-        <v>0.932358583868663</v>
+        <v>0.9961762476863529</v>
       </c>
       <c r="V2" t="n">
         <v>1.182935915054998</v>

</xml_diff>

<commit_message>
Update the Logs Parameter
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_MACD.xlsx
+++ b/Data/binance_ETHUSDT_MACD.xlsx
@@ -507,12 +507,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>460.49000000</t>
+          <t>460.30000000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>57065.32063000</t>
+          <t>60990.93425000</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -520,20 +520,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>26239302.98475610</t>
+          <t>28046266.48769820</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>26968</v>
+        <v>29177</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>32195.65214000</t>
+          <t>34263.14678000</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>14802288.18198700</t>
+          <t>15753973.35760490</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -552,13 +552,13 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>1.932993639696519</v>
+        <v>1.917836944539829</v>
       </c>
       <c r="Q2" t="n">
-        <v>3.698211108460407</v>
+        <v>3.695179769429068</v>
       </c>
       <c r="R2" t="n">
-        <v>-1.765217468763887</v>
+        <v>-1.77734282488924</v>
       </c>
       <c r="S2" t="n">
         <v>5.403876830579691</v>

</xml_diff>

<commit_message>
Clean some old Data and csv file
</commit_message>
<xml_diff>
--- a/Data/binance_ETHUSDT_MACD.xlsx
+++ b/Data/binance_ETHUSDT_MACD.xlsx
@@ -507,12 +507,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>460.30000000</t>
+          <t>460.10000000</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>60990.93425000</t>
+          <t>61436.50791000</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -520,20 +520,20 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>28046266.48769820</t>
+          <t>28251417.94090800</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>29177</v>
+        <v>29421</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>34263.14678000</t>
+          <t>34483.75443000</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>15753973.35760490</t>
+          <t>15855524.12276050</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -552,13 +552,13 @@
         </is>
       </c>
       <c r="P2" t="n">
-        <v>1.917836944539829</v>
+        <v>1.901882528585418</v>
       </c>
       <c r="Q2" t="n">
-        <v>3.695179769429068</v>
+        <v>3.691988886238186</v>
       </c>
       <c r="R2" t="n">
-        <v>-1.77734282488924</v>
+        <v>-1.790106357652768</v>
       </c>
       <c r="S2" t="n">
         <v>5.403876830579691</v>

</xml_diff>